<commit_message>
Added console and some minor changes
</commit_message>
<xml_diff>
--- a/Libraries_for_GAM_and_other_Projects_-_V2.xlsx
+++ b/Libraries_for_GAM_and_other_Projects_-_V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GAM200\Gam200---Sunrise-Studios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C22153B-DFB4-4CB2-B6AC-77EE82A160FD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BAB2DD5-5A03-4315-9DA5-19C904D3D235}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -687,7 +687,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -702,6 +702,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1007,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1793,23 +1797,23 @@
         <v>146</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:6" s="11" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F40" s="3" t="s">
+      <c r="E40" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F40" s="10" t="s">
         <v>160</v>
       </c>
     </row>

</xml_diff>